<commit_message>
+ friday midday uncommited
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="15315" windowHeight="5955" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="15315" windowHeight="5955" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="yudb_outdoor_raw" sheetId="1" state="hidden" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="111">
   <si>
     <t>P1020171</t>
   </si>
@@ -3332,6 +3332,707 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="ru-RU"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Mean vs X</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>yudb_indoor_charts!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>x</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>yudb_indoor_charts!$V$2:$V$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2.3480428686749899E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.7891017076450565E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.19343399128422614</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.28897696549200175</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.38451993969977732</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.4800629139075529</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.57560588811532842</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.671148862323104</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>yudb_indoor_charts!$G$2:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>yudb_indoor_charts!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>mean vs x</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>yudb_indoor_charts!$V$2:$V$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>2.3480428686749899E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.7891017076450565E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.19343399128422614</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.28897696549200175</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.38451993969977732</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.4800629139075529</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.57560588811532842</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.671148862323104</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>yudb_indoor_charts!$K$2:$K$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="121178752"/>
+        <c:axId val="121184640"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="121178752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="121184640"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="121184640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="121178752"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="ru-RU"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Mean vs Y</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>yudb_indoor_charts!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>y</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>yudb_indoor_charts!$W$2:$W$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>6.5076894471688303E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.10209459388076343</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.19768149831435805</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.29326840274795263</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.38885530718154726</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.48444221161514189</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.58002911604873642</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.67561602048233105</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>yudb_indoor_charts!$H$2:$H$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Mean vs Y</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>yudb_indoor_charts!$W$2:$W$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>6.5076894471688303E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.10209459388076343</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.19768149831435805</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.29326840274795263</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.38885530718154726</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.48444221161514189</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.58002911604873642</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.67561602048233105</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>yudb_indoor_charts!$L$2:$L$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="121193600"/>
+        <c:axId val="121195136"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="121193600"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="121195136"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="121195136"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="121193600"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="ru-RU"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Mean vs Z</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>yudb_indoor_charts!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>z</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>yudb_indoor_charts!$X$2:$X$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.35598949424413E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.1688091446884687E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.9816287951328067E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.12794448445577147</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.16607268096021485</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.20420087746465823</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.24232907396910164</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.28045727047354502</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>yudb_indoor_charts!$I$2:$I$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Mean vs Z</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>yudb_indoor_charts!$X$2:$X$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.35598949424413E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.1688091446884687E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.9816287951328067E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.12794448445577147</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.16607268096021485</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.20420087746465823</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.24232907396910164</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.28045727047354502</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>yudb_indoor_charts!$M$2:$M$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="121220096"/>
+        <c:axId val="121230080"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="121220096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="121230080"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="121230080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="121220096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -3442,15 +4143,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>530679</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>176894</xdr:rowOff>
+      <xdr:colOff>517072</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>68037</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>95251</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>13607</xdr:rowOff>
+      <xdr:colOff>81644</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3471,16 +4172,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>557894</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>40823</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>421822</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>54431</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>231323</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>122465</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>95251</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>136073</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3501,20 +4202,115 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>530681</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>163286</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>149681</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>54429</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>204110</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>54428</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>435431</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>136071</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="6" name="Диаграмма 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>517071</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>81643</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>27213</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Диаграмма 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>136073</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>54429</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>27215</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Диаграмма 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>272145</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>136070</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>557895</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>27212</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Диаграмма 3"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -7225,8 +8021,8 @@
   </sheetPr>
   <dimension ref="A1:Y58"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9544,8 +10340,8 @@
   </sheetPr>
   <dimension ref="A1:Y46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F9"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9563,6 +10359,27 @@
       <c r="E1" t="s">
         <v>62</v>
       </c>
+      <c r="G1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" t="s">
+        <v>63</v>
+      </c>
+      <c r="L1" t="s">
+        <v>64</v>
+      </c>
+      <c r="M1" t="s">
+        <v>65</v>
+      </c>
       <c r="P1">
         <v>7</v>
       </c>
@@ -9603,6 +10420,34 @@
       <c r="F2">
         <v>0</v>
       </c>
+      <c r="G2">
+        <f t="array" ref="G2:G10">FREQUENCY(B$2:B$46, V$2:V$9)</f>
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <f t="array" ref="H2:H10">FREQUENCY(C$2:C$46, W$2:W$9)</f>
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <f t="array" ref="I2:I10">FREQUENCY(D$2:D$46, X$2:X$9)</f>
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <f t="array" ref="J2:J10">FREQUENCY(E$2:E$46, Y$2:Y$9)</f>
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <f t="array" ref="K2:K10">FREQUENCY($E$2:$E$46, V$2:V$9)</f>
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <f t="array" ref="L2:L10">FREQUENCY($E$2:$E$46, W$2:W$9)</f>
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <f t="array" ref="M2:M10">FREQUENCY($E$2:$E$46, X$2:X$9)</f>
+        <v>1</v>
+      </c>
       <c r="Q2">
         <f>MAX(B$2:B$46)</f>
         <v>0.671148862323104</v>
@@ -9656,6 +10501,27 @@
       <c r="F3">
         <v>1</v>
       </c>
+      <c r="G3">
+        <v>37</v>
+      </c>
+      <c r="H3">
+        <v>30</v>
+      </c>
+      <c r="I3">
+        <v>22</v>
+      </c>
+      <c r="J3">
+        <v>31</v>
+      </c>
+      <c r="K3">
+        <v>34</v>
+      </c>
+      <c r="L3">
+        <v>34</v>
+      </c>
+      <c r="M3">
+        <v>18</v>
+      </c>
       <c r="Q3">
         <f>(Q2 - Q1) /$P$1</f>
         <v>9.5542974207775577E-2</v>
@@ -9709,6 +10575,27 @@
       <c r="F4">
         <v>2</v>
       </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>7</v>
+      </c>
+      <c r="I4">
+        <v>10</v>
+      </c>
+      <c r="J4">
+        <v>8</v>
+      </c>
+      <c r="K4">
+        <v>6</v>
+      </c>
+      <c r="L4">
+        <v>6</v>
+      </c>
+      <c r="M4">
+        <v>14</v>
+      </c>
       <c r="V4">
         <f>Q$1 +Q$3 * $F4</f>
         <v>0.19343399128422614</v>
@@ -9746,6 +10633,27 @@
       <c r="F5">
         <v>3</v>
       </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="J5">
+        <v>2</v>
+      </c>
+      <c r="K5">
+        <v>3</v>
+      </c>
+      <c r="L5">
+        <v>3</v>
+      </c>
+      <c r="M5">
+        <v>2</v>
+      </c>
       <c r="V5">
         <f>Q$1 +Q$3 * $F5</f>
         <v>0.28897696549200175</v>
@@ -9783,6 +10691,27 @@
       <c r="F6">
         <v>4</v>
       </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>3</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>5</v>
+      </c>
       <c r="V6">
         <f>Q$1 +Q$3 * $F6</f>
         <v>0.38451993969977732</v>
@@ -9820,6 +10749,27 @@
       <c r="F7">
         <v>5</v>
       </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
       <c r="V7">
         <f>Q$1 +Q$3 * $F7</f>
         <v>0.4800629139075529</v>
@@ -9857,6 +10807,27 @@
       <c r="F8">
         <v>6</v>
       </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>2</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>2</v>
+      </c>
       <c r="V8">
         <f>Q$1 +Q$3 * $F8</f>
         <v>0.57560588811532842</v>
@@ -9894,6 +10865,27 @@
       <c r="F9">
         <v>7</v>
       </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>3</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
       <c r="V9">
         <f>Q$1 +Q$3 * $F9</f>
         <v>0.671148862323104</v>
@@ -9928,6 +10920,27 @@
         <f t="shared" si="2"/>
         <v>1.079668556533781E-2</v>
       </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:25">
       <c r="A11" t="s">
@@ -10579,5 +11592,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
+ tuesday midday presentation & stat charts again
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -4,25 +4,27 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="15315" windowHeight="5955" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="15315" windowHeight="5955" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="yudb_outdoor_raw" sheetId="1" state="hidden" r:id="rId1"/>
     <sheet name="yudb_outdoor_interm" sheetId="2" state="hidden" r:id="rId2"/>
-    <sheet name="yudb_outdoor_forMe" sheetId="5" state="hidden" r:id="rId3"/>
+    <sheet name="yudb_outdoor_3axis" sheetId="5" r:id="rId3"/>
     <sheet name="yudb_outdoor_charts" sheetId="4" r:id="rId4"/>
     <sheet name="yudb_indoor_raw" sheetId="3" state="hidden" r:id="rId5"/>
-    <sheet name="yudb_indoor_charts" sheetId="6" r:id="rId6"/>
+    <sheet name="yudb_indoor_3axis" sheetId="7" r:id="rId6"/>
+    <sheet name="yudb_indoor_charts" sheetId="6" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">yudb_indoor_charts!$A$2:$E$46</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">yudb_indoor_3axis!$A$2:$E$46</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">yudb_indoor_charts!$A$2:$E$46</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="114">
   <si>
     <t>P1020171</t>
   </si>
@@ -356,6 +358,15 @@
   <si>
     <t>P1080092</t>
   </si>
+  <si>
+    <t>ось X</t>
+  </si>
+  <si>
+    <t>ось Y</t>
+  </si>
+  <si>
+    <t>ось Z</t>
+  </si>
 </sst>
 </file>
 
@@ -1070,6 +1081,237 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="ru-RU"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Mean vs Z</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>yudb_indoor_charts!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>z</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>yudb_indoor_charts!$X$2:$X$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.77692475084267687</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.9615094909927411</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.146094231142806</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.3306789712928699</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.5152637114429339</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.699848451592999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13.884433191743062</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16.069017931893129</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>yudb_indoor_charts!$I$2:$I$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Mean vs Z</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>yudb_indoor_charts!$X$2:$X$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.77692475084267687</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.9615094909927411</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.146094231142806</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.3306789712928699</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.5152637114429339</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.699848451592999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13.884433191743062</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16.069017931893129</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>yudb_indoor_charts!$M$2:$M$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="75421184"/>
+        <c:axId val="75422720"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="75421184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="75422720"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="75422720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="75421184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="ru-RU"/>
@@ -2247,6 +2489,29 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="ru-RU"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ru-RU"/>
+              <a:t>Диаграмма распределения углов абсолютного отклонения осей координат</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ru-RU" baseline="0"/>
+              <a:t> от верных значений</a:t>
+            </a:r>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -2256,51 +2521,51 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>yudb_outdoor_forMe!$G$1</c:f>
+              <c:f>yudb_outdoor_3axis!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>x</c:v>
+                  <c:v>ось X</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>yudb_outdoor_forMe!$F$2:$F$10</c:f>
+              <c:f>yudb_outdoor_3axis!$F$2:$F$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>6.8800076479676999E-3</c:v>
+                  <c:v>0.39419540124627744</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.12288615158905859</c:v>
+                  <c:v>7.0408578466579126</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.23889229553014948</c:v>
+                  <c:v>13.687520292069546</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.35489843947124039</c:v>
+                  <c:v>20.334182737481182</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.47090458341233127</c:v>
+                  <c:v>26.980845182892818</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.5869107273534222</c:v>
+                  <c:v>33.62750762830445</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.70291687129451308</c:v>
+                  <c:v>40.274170073716085</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.81892301523560396</c:v>
+                  <c:v>46.920832519127721</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>yudb_outdoor_forMe!$G$2:$G$10</c:f>
+              <c:f>yudb_outdoor_3axis!$G$2:$G$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -2341,51 +2606,51 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>yudb_outdoor_forMe!$H$1</c:f>
+              <c:f>yudb_outdoor_3axis!$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>y</c:v>
+                  <c:v>ось Y</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>yudb_outdoor_forMe!$F$2:$F$10</c:f>
+              <c:f>yudb_outdoor_3axis!$F$2:$F$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>6.8800076479676999E-3</c:v>
+                  <c:v>0.39419540124627744</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.12288615158905859</c:v>
+                  <c:v>7.0408578466579126</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.23889229553014948</c:v>
+                  <c:v>13.687520292069546</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.35489843947124039</c:v>
+                  <c:v>20.334182737481182</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.47090458341233127</c:v>
+                  <c:v>26.980845182892818</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.5869107273534222</c:v>
+                  <c:v>33.62750762830445</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.70291687129451308</c:v>
+                  <c:v>40.274170073716085</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.81892301523560396</c:v>
+                  <c:v>46.920832519127721</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>yudb_outdoor_forMe!$H$2:$H$10</c:f>
+              <c:f>yudb_outdoor_3axis!$H$2:$H$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -2426,51 +2691,51 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>yudb_outdoor_forMe!$I$1</c:f>
+              <c:f>yudb_outdoor_3axis!$I$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>z</c:v>
+                  <c:v>ось Z</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>yudb_outdoor_forMe!$F$2:$F$10</c:f>
+              <c:f>yudb_outdoor_3axis!$F$2:$F$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>6.8800076479676999E-3</c:v>
+                  <c:v>0.39419540124627744</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.12288615158905859</c:v>
+                  <c:v>7.0408578466579126</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.23889229553014948</c:v>
+                  <c:v>13.687520292069546</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.35489843947124039</c:v>
+                  <c:v>20.334182737481182</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.47090458341233127</c:v>
+                  <c:v>26.980845182892818</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.5869107273534222</c:v>
+                  <c:v>33.62750762830445</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.70291687129451308</c:v>
+                  <c:v>40.274170073716085</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.81892301523560396</c:v>
+                  <c:v>46.920832519127721</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>yudb_outdoor_forMe!$I$2:$I$10</c:f>
+              <c:f>yudb_outdoor_3axis!$I$2:$I$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -2506,91 +2771,9 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>yudb_outdoor_forMe!$J$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>mean</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:xVal>
-            <c:numRef>
-              <c:f>yudb_outdoor_forMe!$F$2:$F$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>6.8800076479676999E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.12288615158905859</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.23889229553014948</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.35489843947124039</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.47090458341233127</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.5869107273534222</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.70291687129451308</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.81892301523560396</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>yudb_outdoor_forMe!$J$2:$J$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="b"/>
+        </c:dLbls>
         <c:axId val="75056256"/>
         <c:axId val="75057792"/>
       </c:scatterChart>
@@ -2600,8 +2783,36 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="ru-RU" sz="1600" b="0"/>
+                  <a:t>Абсолютная величина угла между вычисленным направлением оси и верным</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="75057792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
@@ -2613,8 +2824,36 @@
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="ru-RU" sz="1600" b="0"/>
+                  <a:t>Количество изображений на интервале</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="75056256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
@@ -2622,12 +2861,23 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400"/>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3348,6 +3598,401 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
+              <a:rPr lang="ru-RU"/>
+              <a:t>Диаграмма распределения углов абсолютного отклонения осей координат</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ru-RU" baseline="0"/>
+              <a:t> от верных значений</a:t>
+            </a:r>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>yudb_indoor_3axis!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ось X</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>yudb_indoor_3axis!$F$2:$F$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.13453294649086753</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.6453063177152787</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.156079688939691</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.666853060164105</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22.177626431388514</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>27.688399802612924</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33.199173173837337</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>38.709946545061747</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>yudb_indoor_3axis!$G$2:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>yudb_indoor_3axis!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ось Y</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>yudb_indoor_3axis!$F$2:$F$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.13453294649086753</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.6453063177152787</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.156079688939691</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.666853060164105</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22.177626431388514</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>27.688399802612924</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33.199173173837337</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>38.709946545061747</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>yudb_indoor_3axis!$H$2:$H$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>yudb_indoor_3axis!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ось Z</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>yudb_indoor_3axis!$F$2:$F$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.13453294649086753</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.6453063177152787</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.156079688939691</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.666853060164105</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22.177626431388514</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>27.688399802612924</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33.199173173837337</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>38.709946545061747</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>yudb_indoor_3axis!$I$2:$I$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="60462208"/>
+        <c:axId val="60463744"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="60462208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="ru-RU" sz="1600" b="0"/>
+                  <a:t>Абсолютная величина угла между вычисленным направлением оси и верным</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="60463744"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="60463744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="ru-RU" sz="1600" b="0"/>
+                  <a:t>Количество изображений на интервале</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="60462208"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400"/>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="ru-RU"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
               <a:rPr lang="en-US"/>
               <a:t>Mean vs X</a:t>
             </a:r>
@@ -3573,7 +4218,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="ru-RU"/>
   <c:chart>
@@ -3786,237 +4431,6 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="75365760"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="ru-RU"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Mean vs Z</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-    </c:title>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>yudb_indoor_charts!$I$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>z</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:xVal>
-            <c:numRef>
-              <c:f>yudb_indoor_charts!$X$2:$X$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>0.77692475084267687</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.9615094909927411</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.146094231142806</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7.3306789712928699</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9.5152637114429339</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>11.699848451592999</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>13.884433191743062</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>16.069017931893129</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>yudb_indoor_charts!$I$2:$I$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Mean vs Z</c:v>
-          </c:tx>
-          <c:xVal>
-            <c:numRef>
-              <c:f>yudb_indoor_charts!$X$2:$X$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>0.77692475084267687</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.9615094909927411</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.146094231142806</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7.3306789712928699</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9.5152637114429339</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>11.699848451592999</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>13.884433191743062</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>16.069017931893129</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>yudb_indoor_charts!$M$2:$M$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:axId val="75421184"/>
-        <c:axId val="75422720"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="75421184"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75422720"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="75422720"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75421184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4109,15 +4523,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>585106</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>217714</xdr:colOff>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>176893</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>530679</xdr:colOff>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>176894</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4236,6 +4650,41 @@
 </file>
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>517073</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>217716</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>95252</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Диаграмма 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -7911,8 +8360,8 @@
   </sheetPr>
   <dimension ref="A1:Q58"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:J10"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7928,13 +8377,13 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>59</v>
+        <v>111</v>
       </c>
       <c r="H1" t="s">
-        <v>60</v>
+        <v>112</v>
       </c>
       <c r="I1" t="s">
-        <v>61</v>
+        <v>113</v>
       </c>
       <c r="J1" t="s">
         <v>62</v>
@@ -7944,7 +8393,7 @@
       </c>
       <c r="Q1">
         <f>MIN(B$2:E$58)</f>
-        <v>6.8800076479676999E-3</v>
+        <v>0.39419540124627744</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -7952,21 +8401,20 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>1.9565232164372101E-2</v>
+        <v>1.1210052282121303</v>
       </c>
       <c r="C2">
-        <v>2.0504633680462798E-2</v>
+        <v>1.1748289703523183</v>
       </c>
       <c r="D2">
-        <v>6.8800076479676999E-3</v>
+        <v>0.39419540124627744</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E33" si="0">SUM(B2:D2) / 3</f>
-        <v>1.5649957830934199E-2</v>
+        <v>0.89667653327024199</v>
       </c>
       <c r="F2">
-        <f t="shared" ref="F2:F9" si="1">Q$1 +Q$3 * $L2</f>
-        <v>6.8800076479676999E-3</v>
+        <f t="shared" ref="F2:F9" si="0">Q$1 +Q$3 * $L2</f>
+        <v>0.39419540124627744</v>
       </c>
       <c r="G2">
         <f t="array" ref="G2:G10">FREQUENCY(B$2:B$58, $F$2:$F$9)</f>
@@ -7989,7 +8437,7 @@
       </c>
       <c r="Q2">
         <f>MAX(B$2:E$58)</f>
-        <v>0.81892301523560396</v>
+        <v>46.920832519127721</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -7997,21 +8445,20 @@
         <v>45</v>
       </c>
       <c r="B3">
-        <v>2.39269954357046E-2</v>
+        <v>1.3709158548946578</v>
       </c>
       <c r="C3">
-        <v>2.46483419890372E-2</v>
+        <v>1.4122459679669244</v>
       </c>
       <c r="D3">
-        <v>2.0721057928858901E-2</v>
+        <v>1.1872291663697059</v>
       </c>
       <c r="E3">
+        <v>1.323463663077096</v>
+      </c>
+      <c r="F3">
         <f t="shared" si="0"/>
-        <v>2.3098798451200234E-2</v>
-      </c>
-      <c r="F3">
-        <f t="shared" si="1"/>
-        <v>0.12288615158905859</v>
+        <v>7.0408578466579126</v>
       </c>
       <c r="G3">
         <v>25</v>
@@ -8030,7 +8477,7 @@
       </c>
       <c r="Q3">
         <f>(Q2 - Q1) /$P$1</f>
-        <v>0.11600614394109089</v>
+        <v>6.6466624454116348</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -8038,21 +8485,20 @@
         <v>47</v>
       </c>
       <c r="B4">
-        <v>3.66924593685636E-2</v>
+        <v>2.1023230617739519</v>
       </c>
       <c r="C4">
-        <v>5.76146126172314E-2</v>
+        <v>3.3010741412485411</v>
       </c>
       <c r="D4">
-        <v>5.9233054651864403E-2</v>
+        <v>3.3938040392195781</v>
       </c>
       <c r="E4">
+        <v>2.9324004140806901</v>
+      </c>
+      <c r="F4">
         <f t="shared" si="0"/>
-        <v>5.118004221255313E-2</v>
-      </c>
-      <c r="F4">
-        <f t="shared" si="1"/>
-        <v>0.23889229553014948</v>
+        <v>13.687520292069546</v>
       </c>
       <c r="G4">
         <v>14</v>
@@ -8075,21 +8521,20 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>2.2261768078036599E-2</v>
+        <v>1.2755053553705593</v>
       </c>
       <c r="C5">
-        <v>7.2214911764759304E-2</v>
+        <v>4.1376096620303437</v>
       </c>
       <c r="D5">
-        <v>7.19410610097099E-2</v>
+        <v>4.1219191695495416</v>
       </c>
       <c r="E5">
+        <v>3.1783447289834816</v>
+      </c>
+      <c r="F5">
         <f t="shared" si="0"/>
-        <v>5.5472580284168599E-2</v>
-      </c>
-      <c r="F5">
-        <f t="shared" si="1"/>
-        <v>0.35489843947124039</v>
+        <v>20.334182737481182</v>
       </c>
       <c r="G5">
         <v>11</v>
@@ -8112,21 +8557,20 @@
         <v>24</v>
       </c>
       <c r="B6">
-        <v>3.0082006759730998E-2</v>
+        <v>1.7235720266165993</v>
       </c>
       <c r="C6">
-        <v>6.6779006376605707E-2</v>
+        <v>3.826155225456719</v>
       </c>
       <c r="D6">
-        <v>7.0493720169324106E-2</v>
+        <v>4.0389926478785183</v>
       </c>
       <c r="E6">
+        <v>3.1962399666506123</v>
+      </c>
+      <c r="F6">
         <f t="shared" si="0"/>
-        <v>5.5784911101886936E-2</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="1"/>
-        <v>0.47090458341233127</v>
+        <v>26.980845182892818</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -8149,21 +8593,20 @@
         <v>20</v>
       </c>
       <c r="B7">
-        <v>1.6814148090813202E-2</v>
+        <v>0.96337972171154729</v>
       </c>
       <c r="C7">
-        <v>8.0282017189908905E-2</v>
+        <v>4.5998207557785058</v>
       </c>
       <c r="D7">
-        <v>7.8877329818613007E-2</v>
+        <v>4.5193380978679247</v>
       </c>
       <c r="E7">
+        <v>3.3608461917859929</v>
+      </c>
+      <c r="F7">
         <f t="shared" si="0"/>
-        <v>5.8657831699778375E-2</v>
-      </c>
-      <c r="F7">
-        <f t="shared" si="1"/>
-        <v>0.5869107273534222</v>
+        <v>33.62750762830445</v>
       </c>
       <c r="G7">
         <v>2</v>
@@ -8186,21 +8629,20 @@
         <v>5</v>
       </c>
       <c r="B8">
-        <v>7.5683786828808802E-2</v>
+        <v>4.3363615628585528</v>
       </c>
       <c r="C8">
-        <v>8.4851547729877894E-2</v>
+        <v>4.8616355700748644</v>
       </c>
       <c r="D8">
-        <v>3.9390816672038698E-2</v>
+        <v>2.2569275468813763</v>
       </c>
       <c r="E8">
+        <v>3.8183082266049313</v>
+      </c>
+      <c r="F8">
         <f t="shared" si="0"/>
-        <v>6.6642050410241793E-2</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="1"/>
-        <v>0.70291687129451308</v>
+        <v>40.274170073716085</v>
       </c>
       <c r="G8">
         <v>2</v>
@@ -8223,21 +8665,20 @@
         <v>4</v>
       </c>
       <c r="B9">
-        <v>3.0169254574166401E-2</v>
+        <v>1.7285709581554884</v>
       </c>
       <c r="C9">
-        <v>8.3159783704202295E-2</v>
+        <v>4.7647046314715906</v>
       </c>
       <c r="D9">
-        <v>8.8365524456744005E-2</v>
+        <v>5.0629716058314882</v>
       </c>
       <c r="E9">
+        <v>3.8520823984861896</v>
+      </c>
+      <c r="F9">
         <f t="shared" si="0"/>
-        <v>6.7231520911704243E-2</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="1"/>
-        <v>0.81892301523560396</v>
+        <v>46.920832519127721</v>
       </c>
       <c r="G9">
         <v>3</v>
@@ -8260,17 +8701,16 @@
         <v>2</v>
       </c>
       <c r="B10">
-        <v>9.6167601568129105E-2</v>
+        <v>5.5099976957494752</v>
       </c>
       <c r="C10">
-        <v>9.5155288001719004E-2</v>
+        <v>5.4519964008503399</v>
       </c>
       <c r="D10">
-        <v>1.44371923784062E-2</v>
+        <v>0.82719019130111426</v>
       </c>
       <c r="E10">
-        <f t="shared" si="0"/>
-        <v>6.858669398275144E-2</v>
+        <v>3.9297280959669765</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -8290,17 +8730,16 @@
         <v>23</v>
       </c>
       <c r="B11">
-        <v>4.0583456342337003E-2</v>
+        <v>2.3252607664693432</v>
       </c>
       <c r="C11">
-        <v>9.3526978512517803E-2</v>
+        <v>5.3587011393780077</v>
       </c>
       <c r="D11">
-        <v>8.8969693113070999E-2</v>
+        <v>5.0975879199531144</v>
       </c>
       <c r="E11">
-        <f t="shared" si="0"/>
-        <v>7.4360042655975275E-2</v>
+        <v>4.260516608600156</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -8308,17 +8747,16 @@
         <v>16</v>
       </c>
       <c r="B12">
-        <v>3.27457523597929E-2</v>
+        <v>1.8761934071966893</v>
       </c>
       <c r="C12">
-        <v>9.9795982111292203E-2</v>
+        <v>5.7178885873401057</v>
       </c>
       <c r="D12">
-        <v>9.4333494032757495E-2</v>
+        <v>5.4049110747995401</v>
       </c>
       <c r="E12">
-        <f t="shared" si="0"/>
-        <v>7.5625076167947544E-2</v>
+        <v>4.3329976897787787</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -8326,17 +8764,16 @@
         <v>9</v>
       </c>
       <c r="B13">
-        <v>9.3622797858686796E-2</v>
+        <v>5.3641911835091944</v>
       </c>
       <c r="C13">
-        <v>6.3894294958753706E-2</v>
+        <v>3.6608734361005997</v>
       </c>
       <c r="D13">
-        <v>8.2641929238977202E-2</v>
+        <v>4.7350337562121894</v>
       </c>
       <c r="E13">
-        <f t="shared" si="0"/>
-        <v>8.005300735213923E-2</v>
+        <v>4.5866994586073275</v>
       </c>
     </row>
     <row r="14" spans="1:17">
@@ -8344,17 +8781,16 @@
         <v>49</v>
       </c>
       <c r="B14">
-        <v>4.7488878854939097E-2</v>
+        <v>2.7209123321960678</v>
       </c>
       <c r="C14">
-        <v>0.104501879711214</v>
+        <v>5.9875166586363679</v>
       </c>
       <c r="D14">
-        <v>9.30709997573963E-2</v>
+        <v>5.3325754811619168</v>
       </c>
       <c r="E14">
-        <f t="shared" si="0"/>
-        <v>8.1687252774516467E-2</v>
+        <v>4.680334823998118</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -8362,17 +8798,16 @@
         <v>55</v>
       </c>
       <c r="B15">
-        <v>4.6248129902809E-2</v>
+        <v>2.6498226538037337</v>
       </c>
       <c r="C15">
-        <v>0.11057809641814099</v>
+        <v>6.3356582313501644</v>
       </c>
       <c r="D15">
-        <v>0.104229179761008</v>
+        <v>5.9718921024161364</v>
       </c>
       <c r="E15">
-        <f t="shared" si="0"/>
-        <v>8.7018468693985995E-2</v>
+        <v>4.9857909958566786</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -8380,17 +8815,16 @@
         <v>35</v>
       </c>
       <c r="B16">
-        <v>8.7191311790792106E-2</v>
+        <v>4.9956941758216393</v>
       </c>
       <c r="C16">
-        <v>0.110418900996724</v>
+        <v>6.3265370055851644</v>
       </c>
       <c r="D16">
-        <v>6.8768314811834597E-2</v>
+        <v>3.9401342029451083</v>
       </c>
       <c r="E16">
-        <f t="shared" si="0"/>
-        <v>8.8792842533116909E-2</v>
+        <v>5.0874551281173046</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -8398,17 +8832,16 @@
         <v>17</v>
       </c>
       <c r="B17">
-        <v>0.122706228786875</v>
+        <v>7.0305490294546251</v>
       </c>
       <c r="C17">
-        <v>0.121454859724503</v>
+        <v>6.9588508635674664</v>
       </c>
       <c r="D17">
-        <v>3.7996491509359097E-2</v>
+        <v>2.1770385997909432</v>
       </c>
       <c r="E17">
-        <f t="shared" si="0"/>
-        <v>9.4052526673579037E-2</v>
+        <v>5.3888128309376784</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -8416,17 +8849,16 @@
         <v>44</v>
       </c>
       <c r="B18">
-        <v>0.107348842734351</v>
+        <v>6.1506356242919242</v>
       </c>
       <c r="C18">
-        <v>0.12727564622609699</v>
+        <v>7.2923573635555217</v>
       </c>
       <c r="D18">
-        <v>6.8330619833880904E-2</v>
+        <v>3.9150561279942901</v>
       </c>
       <c r="E18">
-        <f t="shared" si="0"/>
-        <v>0.1009850362647763</v>
+        <v>5.7860163719472455</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -8434,17 +8866,16 @@
         <v>48</v>
       </c>
       <c r="B19">
-        <v>5.9514295458887402E-2</v>
+        <v>3.409917950488849</v>
       </c>
       <c r="C19">
-        <v>0.16218629449737401</v>
+        <v>9.2925901695653774</v>
       </c>
       <c r="D19">
-        <v>0.151039451347665</v>
+        <v>8.6539231021927385</v>
       </c>
       <c r="E19">
-        <f t="shared" si="0"/>
-        <v>0.12424668043464214</v>
+        <v>7.1188104074156557</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -8452,17 +8883,16 @@
         <v>33</v>
       </c>
       <c r="B20">
-        <v>7.5709840070607506E-2</v>
+        <v>4.3378543036562531</v>
       </c>
       <c r="C20">
-        <v>0.15839073659813999</v>
+        <v>9.0751207210417277</v>
       </c>
       <c r="D20">
-        <v>0.13999091983613099</v>
+        <v>8.020888876764543</v>
       </c>
       <c r="E20">
-        <f t="shared" si="0"/>
-        <v>0.12469716550162617</v>
+        <v>7.1446213004875085</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -8470,17 +8900,16 @@
         <v>22</v>
       </c>
       <c r="B21">
-        <v>0.12621343014479899</v>
+        <v>7.2314968651662213</v>
       </c>
       <c r="C21">
-        <v>9.1855048421483398E-2</v>
+        <v>5.2629066015208137</v>
       </c>
       <c r="D21">
-        <v>0.15608016346148901</v>
+        <v>8.9427346320553216</v>
       </c>
       <c r="E21">
-        <f t="shared" si="0"/>
-        <v>0.12471621400925714</v>
+        <v>7.1457126995807858</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -8488,17 +8917,16 @@
         <v>3</v>
       </c>
       <c r="B22">
-        <v>0.14864168688182</v>
+        <v>8.5165413180333793</v>
       </c>
       <c r="C22">
-        <v>0.16165960480956501</v>
+        <v>9.2624130733408592</v>
       </c>
       <c r="D22">
-        <v>0.111345291278063</v>
+        <v>6.3796152588878261</v>
       </c>
       <c r="E22">
-        <f t="shared" si="0"/>
-        <v>0.140548860989816</v>
+        <v>8.0528565500873555</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -8506,17 +8934,16 @@
         <v>15</v>
       </c>
       <c r="B23">
-        <v>0.115076885759176</v>
+        <v>6.5934198735099114</v>
       </c>
       <c r="C23">
-        <v>0.173090065815034</v>
+        <v>9.9173302468430968</v>
       </c>
       <c r="D23">
-        <v>0.13595621083047099</v>
+        <v>7.7897170791768007</v>
       </c>
       <c r="E23">
-        <f t="shared" si="0"/>
-        <v>0.141374387468227</v>
+        <v>8.100155733176603</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -8524,17 +8951,16 @@
         <v>40</v>
       </c>
       <c r="B24">
-        <v>0.12155871504374</v>
+        <v>6.9648013350397298</v>
       </c>
       <c r="C24">
-        <v>0.176161646036017</v>
+        <v>10.093318829941282</v>
       </c>
       <c r="D24">
-        <v>0.127361747547523</v>
+        <v>7.297290605883731</v>
       </c>
       <c r="E24">
-        <f t="shared" si="0"/>
-        <v>0.14169403620909332</v>
+        <v>8.1184702569549145</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -8542,17 +8968,16 @@
         <v>26</v>
       </c>
       <c r="B25">
-        <v>0.175035288820028</v>
+        <v>10.028783315241007</v>
       </c>
       <c r="C25">
-        <v>8.7620683330971602E-2</v>
+        <v>5.0202953529169569</v>
       </c>
       <c r="D25">
-        <v>0.18549753299198199</v>
+        <v>10.628225750529314</v>
       </c>
       <c r="E25">
-        <f t="shared" si="0"/>
-        <v>0.14938450171432718</v>
+        <v>8.5591014728957582</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -8560,17 +8985,16 @@
         <v>42</v>
       </c>
       <c r="B26">
-        <v>0.165511964699155</v>
+        <v>9.4831370361798495</v>
       </c>
       <c r="C26">
-        <v>0.18654840809932799</v>
+        <v>10.688436458975596</v>
       </c>
       <c r="D26">
-        <v>9.8985878863429605E-2</v>
+        <v>5.6714730902677388</v>
       </c>
       <c r="E26">
-        <f t="shared" si="0"/>
-        <v>0.15034875055397087</v>
+        <v>8.6143488618077289</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -8578,17 +9002,16 @@
         <v>36</v>
       </c>
       <c r="B27">
-        <v>8.8041174508344394E-2</v>
+        <v>5.0443877227029041</v>
       </c>
       <c r="C27">
-        <v>0.207943627654575</v>
+        <v>11.914292241247017</v>
       </c>
       <c r="D27">
-        <v>0.18893162605986799</v>
+        <v>10.824984789774314</v>
       </c>
       <c r="E27">
-        <f t="shared" si="0"/>
-        <v>0.16163880940759578</v>
+        <v>9.261221584574745</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -8596,17 +9019,16 @@
         <v>32</v>
       </c>
       <c r="B28">
-        <v>9.5266877484380896E-2</v>
+        <v>5.4583900072449145</v>
       </c>
       <c r="C28">
-        <v>0.21538556760368799</v>
+        <v>12.340683991720994</v>
       </c>
       <c r="D28">
-        <v>0.19455494375698401</v>
+        <v>11.147177160680288</v>
       </c>
       <c r="E28">
-        <f t="shared" si="0"/>
-        <v>0.16840246294835096</v>
+        <v>9.6487503865487323</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -8614,17 +9036,16 @@
         <v>50</v>
       </c>
       <c r="B29">
-        <v>0.15290151341855299</v>
+        <v>8.7606114000460096</v>
       </c>
       <c r="C29">
-        <v>0.24298595276132601</v>
+        <v>13.922069574189171</v>
       </c>
       <c r="D29">
-        <v>0.188616467666125</v>
+        <v>10.806927543934719</v>
       </c>
       <c r="E29">
-        <f t="shared" si="0"/>
-        <v>0.1948346446153347</v>
+        <v>11.163202839389969</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -8632,17 +9053,16 @@
         <v>43</v>
       </c>
       <c r="B30">
-        <v>9.8560076810135705E-2</v>
+        <v>5.6470764297059937</v>
       </c>
       <c r="C30">
-        <v>0.26286133372432902</v>
+        <v>15.060845019583907</v>
       </c>
       <c r="D30">
-        <v>0.24356413354249201</v>
+        <v>13.95519689274556</v>
       </c>
       <c r="E30">
-        <f t="shared" si="0"/>
-        <v>0.20166184802565223</v>
+        <v>11.554372780678486</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -8650,17 +9070,16 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>0.29159614975891102</v>
+        <v>16.707228703450298</v>
       </c>
       <c r="C31">
-        <v>0.29133131747289198</v>
+        <v>16.692054931182607</v>
       </c>
       <c r="D31">
-        <v>3.4580700295362102E-2</v>
+        <v>1.9813281795310478</v>
       </c>
       <c r="E31">
-        <f t="shared" si="0"/>
-        <v>0.20583605584238837</v>
+        <v>11.793537271387985</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -8668,17 +9087,16 @@
         <v>27</v>
       </c>
       <c r="B32">
-        <v>0.16819822606655599</v>
+        <v>9.6370484752009684</v>
       </c>
       <c r="C32">
-        <v>0.26737186595878798</v>
+        <v>15.319279479976117</v>
       </c>
       <c r="D32">
-        <v>0.20756249457879999</v>
+        <v>11.89245492457227</v>
       </c>
       <c r="E32">
-        <f t="shared" si="0"/>
-        <v>0.21437752886804798</v>
+        <v>12.282927626583117</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -8686,17 +9104,16 @@
         <v>39</v>
       </c>
       <c r="B33">
-        <v>0.258110132106037</v>
+        <v>14.788621219240047</v>
       </c>
       <c r="C33">
-        <v>0.27595097695689502</v>
+        <v>15.810826332141918</v>
       </c>
       <c r="D33">
-        <v>0.109796555689871</v>
+        <v>6.2908792461027128</v>
       </c>
       <c r="E33">
-        <f t="shared" si="0"/>
-        <v>0.21461922158426769</v>
+        <v>12.29677559916156</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -8704,17 +9121,16 @@
         <v>25</v>
       </c>
       <c r="B34">
-        <v>7.7253112427583606E-2</v>
+        <v>4.4262772963501904</v>
       </c>
       <c r="C34">
-        <v>0.30196094259784101</v>
+        <v>17.301087588648407</v>
       </c>
       <c r="D34">
-        <v>0.29191796211861498</v>
+        <v>16.725667193456481</v>
       </c>
       <c r="E34">
-        <f t="shared" ref="E34:E65" si="2">SUM(B34:D34) / 3</f>
-        <v>0.22371067238134654</v>
+        <v>12.817677359485026</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -8722,17 +9138,16 @@
         <v>13</v>
       </c>
       <c r="B35">
-        <v>0.193348247204187</v>
+        <v>11.078038541052035</v>
       </c>
       <c r="C35">
-        <v>0.27888675052386402</v>
+        <v>15.979033767135309</v>
       </c>
       <c r="D35">
-        <v>0.20035461640205399</v>
+        <v>11.479473925800272</v>
       </c>
       <c r="E35">
-        <f t="shared" si="2"/>
-        <v>0.22419653804336834</v>
+        <v>12.845515411329206</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -8740,17 +9155,16 @@
         <v>52</v>
       </c>
       <c r="B36">
-        <v>0.123909383225261</v>
+        <v>7.0994847008765758</v>
       </c>
       <c r="C36">
-        <v>0.29203437299271401</v>
+        <v>16.732337045231784</v>
       </c>
       <c r="D36">
-        <v>0.26439120745510603</v>
+        <v>15.148500327545362</v>
       </c>
       <c r="E36">
-        <f t="shared" si="2"/>
-        <v>0.22677832122436037</v>
+        <v>12.993440691217909</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -8758,17 +9172,16 @@
         <v>19</v>
       </c>
       <c r="B37">
-        <v>0.24688866161589701</v>
+        <v>14.145678320224427</v>
       </c>
       <c r="C37">
-        <v>0.28773430175234899</v>
+        <v>16.485961111553284</v>
       </c>
       <c r="D37">
-        <v>0.147846183179939</v>
+        <v>8.470962313328565</v>
       </c>
       <c r="E37">
-        <f t="shared" si="2"/>
-        <v>0.22748971551606167</v>
+        <v>13.034200581702093</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -8776,17 +9189,16 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>0.214882714471054</v>
+        <v>12.311872629506134</v>
       </c>
       <c r="C38">
-        <v>0.28337538305940801</v>
+        <v>16.236213467207087</v>
       </c>
       <c r="D38">
-        <v>0.184359307759838</v>
+        <v>10.563010248592166</v>
       </c>
       <c r="E38">
-        <f t="shared" si="2"/>
-        <v>0.22753913509676668</v>
+        <v>13.037032115101795</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -8794,17 +9206,16 @@
         <v>54</v>
       </c>
       <c r="B39">
-        <v>0.242914462611554</v>
+        <v>13.917973490330478</v>
       </c>
       <c r="C39">
-        <v>0.293884336426813</v>
+        <v>16.838332142259183</v>
       </c>
       <c r="D39">
-        <v>0.170015739317874</v>
+        <v>9.7411843137105905</v>
       </c>
       <c r="E39">
-        <f t="shared" si="2"/>
-        <v>0.23560484611874699</v>
+        <v>13.499163315433417</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -8812,17 +9223,16 @@
         <v>56</v>
       </c>
       <c r="B40">
-        <v>0.23128286703943601</v>
+        <v>13.25153215504506</v>
       </c>
       <c r="C40">
-        <v>0.30534264327565902</v>
+        <v>17.49484476506391</v>
       </c>
       <c r="D40">
-        <v>0.209546718062712</v>
+        <v>12.006142555811172</v>
       </c>
       <c r="E40">
-        <f t="shared" si="2"/>
-        <v>0.24872407612593564</v>
+        <v>14.250839825306711</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -8830,17 +9240,16 @@
         <v>12</v>
       </c>
       <c r="B41">
-        <v>0.216039771625544</v>
+        <v>12.378167121113828</v>
       </c>
       <c r="C41">
-        <v>0.310784984669217</v>
+        <v>17.806667957584128</v>
       </c>
       <c r="D41">
-        <v>0.22329857609460799</v>
+        <v>12.794065981501895</v>
       </c>
       <c r="E41">
-        <f t="shared" si="2"/>
-        <v>0.25004111079645636</v>
+        <v>14.326300353399951</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -8848,17 +9257,16 @@
         <v>31</v>
       </c>
       <c r="B42">
-        <v>0.167131313163075</v>
+        <v>9.5759188687234591</v>
       </c>
       <c r="C42">
-        <v>0.31656823120362299</v>
+        <v>18.13802357588925</v>
       </c>
       <c r="D42">
-        <v>0.27034538822387</v>
+        <v>15.489649756053497</v>
       </c>
       <c r="E42">
-        <f t="shared" si="2"/>
-        <v>0.25134831086352266</v>
+        <v>14.401197400222069</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -8866,17 +9274,16 @@
         <v>34</v>
       </c>
       <c r="B43">
-        <v>0.32078505465655399</v>
+        <v>18.37962976269398</v>
       </c>
       <c r="C43">
-        <v>0.33455041684435999</v>
+        <v>19.168326919524233</v>
       </c>
       <c r="D43">
-        <v>0.108127159858925</v>
+        <v>6.1952299106527722</v>
       </c>
       <c r="E43">
-        <f t="shared" si="2"/>
-        <v>0.25448754378661298</v>
+        <v>14.581062197623661</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -8884,17 +9291,16 @@
         <v>51</v>
       </c>
       <c r="B44">
-        <v>0.228786904505591</v>
+        <v>13.108524036032962</v>
       </c>
       <c r="C44">
-        <v>0.321287544273403</v>
+        <v>18.408420296988574</v>
       </c>
       <c r="D44">
-        <v>0.225068956141243</v>
+        <v>12.895501286308255</v>
       </c>
       <c r="E44">
-        <f t="shared" si="2"/>
-        <v>0.25838113497341236</v>
+        <v>14.804148539776598</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -8902,17 +9308,16 @@
         <v>18</v>
       </c>
       <c r="B45">
-        <v>0.31424584817048701</v>
+        <v>18.004960829677767</v>
       </c>
       <c r="C45">
-        <v>0.135753043747423</v>
+        <v>7.7780764627821668</v>
       </c>
       <c r="D45">
-        <v>0.33582661427002503</v>
+        <v>19.241447645840299</v>
       </c>
       <c r="E45">
-        <f t="shared" si="2"/>
-        <v>0.26194183539597832</v>
+        <v>15.008161646100076</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -8920,17 +9325,16 @@
         <v>28</v>
       </c>
       <c r="B46">
-        <v>0.25617902336799397</v>
+        <v>14.677976838769347</v>
       </c>
       <c r="C46">
-        <v>0.34703512730541403</v>
+        <v>19.883648137385457</v>
       </c>
       <c r="D46">
-        <v>0.233515143905453</v>
+        <v>13.379432198172525</v>
       </c>
       <c r="E46">
-        <f t="shared" si="2"/>
-        <v>0.27890976485962032</v>
+        <v>15.980352391442443</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -8938,17 +9342,16 @@
         <v>38</v>
       </c>
       <c r="B47">
-        <v>0.319790218329562</v>
+        <v>18.322629839851043</v>
       </c>
       <c r="C47">
-        <v>0.36564931715135601</v>
+        <v>20.950162654613205</v>
       </c>
       <c r="D47">
-        <v>0.17628096565323001</v>
+        <v>10.100155340420704</v>
       </c>
       <c r="E47">
-        <f t="shared" si="2"/>
-        <v>0.287240167044716</v>
+        <v>16.457649278294983</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -8956,17 +9359,16 @@
         <v>53</v>
       </c>
       <c r="B48">
-        <v>0.32130013957834302</v>
+        <v>18.409141954803317</v>
       </c>
       <c r="C48">
-        <v>0.25325499106434302</v>
+        <v>14.510442128610231</v>
       </c>
       <c r="D48">
-        <v>0.33475798981312199</v>
+        <v>19.180219974575294</v>
       </c>
       <c r="E48">
-        <f t="shared" si="2"/>
-        <v>0.30310437348526936</v>
+        <v>17.366601352662951</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -8974,17 +9376,16 @@
         <v>6</v>
       </c>
       <c r="B49">
-        <v>0.34574875527850901</v>
+        <v>19.80994444936011</v>
       </c>
       <c r="C49">
-        <v>0.40185611629226797</v>
+        <v>23.024659435065356</v>
       </c>
       <c r="D49">
-        <v>0.205591313462125</v>
+        <v>11.779514565930908</v>
       </c>
       <c r="E49">
-        <f t="shared" si="2"/>
-        <v>0.31773206167763401</v>
+        <v>18.204706150118792</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -8992,17 +9393,16 @@
         <v>1</v>
       </c>
       <c r="B50">
-        <v>0.21363980518192799</v>
+        <v>12.240659172921609</v>
       </c>
       <c r="C50">
-        <v>0.45062464983771799</v>
+        <v>25.818890580261819</v>
       </c>
       <c r="D50">
-        <v>0.395353600443624</v>
+        <v>22.652092720721125</v>
       </c>
       <c r="E50">
-        <f t="shared" si="2"/>
-        <v>0.35320601848775662</v>
+        <v>20.237214157968182</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -9010,17 +9410,16 @@
         <v>29</v>
       </c>
       <c r="B51">
-        <v>0.27420464056208199</v>
+        <v>15.71076862710904</v>
       </c>
       <c r="C51">
-        <v>0.46780167059264799</v>
+        <v>26.803061374127925</v>
       </c>
       <c r="D51">
-        <v>0.37815204027779797</v>
+        <v>21.666515922178938</v>
       </c>
       <c r="E51">
-        <f t="shared" si="2"/>
-        <v>0.37338611714417597</v>
+        <v>21.393448641138633</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -9028,17 +9427,16 @@
         <v>41</v>
       </c>
       <c r="B52">
-        <v>0.50456430143220399</v>
+        <v>28.909404965031968</v>
       </c>
       <c r="C52">
-        <v>0.169445604839324</v>
+        <v>9.708518014334782</v>
       </c>
       <c r="D52">
-        <v>0.47980279009076598</v>
+        <v>27.490674870802248</v>
       </c>
       <c r="E52">
-        <f t="shared" si="2"/>
-        <v>0.38460423212076461</v>
+        <v>22.036199283389664</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -9046,17 +9444,16 @@
         <v>46</v>
       </c>
       <c r="B53">
-        <v>0.60159841243019796</v>
+        <v>34.469049994020985</v>
       </c>
       <c r="C53">
-        <v>6.2298860167010202E-2</v>
+        <v>3.5694617560453636</v>
       </c>
       <c r="D53">
-        <v>0.60164343165351997</v>
+        <v>34.471629405514292</v>
       </c>
       <c r="E53">
-        <f t="shared" si="2"/>
-        <v>0.42184690141690934</v>
+        <v>24.170047051860212</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -9064,17 +9461,16 @@
         <v>21</v>
       </c>
       <c r="B54">
-        <v>0.61559888504547799</v>
+        <v>35.271217986065018</v>
       </c>
       <c r="C54">
-        <v>0.20008680641600099</v>
+        <v>11.464129543887978</v>
       </c>
       <c r="D54">
-        <v>0.60068362841715806</v>
+        <v>34.416636730907761</v>
       </c>
       <c r="E54">
-        <f t="shared" si="2"/>
-        <v>0.47212310662621232</v>
+        <v>27.050661420286918</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -9082,17 +9478,16 @@
         <v>0</v>
       </c>
       <c r="B55">
-        <v>0.56144638587108397</v>
+        <v>32.168508333286567</v>
       </c>
       <c r="C55">
-        <v>0.35368944834274602</v>
+        <v>20.264912648349696</v>
       </c>
       <c r="D55">
-        <v>0.56293994201440001</v>
+        <v>32.254082796764408</v>
       </c>
       <c r="E55">
-        <f t="shared" si="2"/>
-        <v>0.49269192540941004</v>
+        <v>28.22916792613356</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -9100,17 +9495,16 @@
         <v>8</v>
       </c>
       <c r="B56">
-        <v>0.72813606806641595</v>
+        <v>41.71912361145607</v>
       </c>
       <c r="C56">
-        <v>5.9118187479932902E-2</v>
+        <v>3.3872226350632992</v>
       </c>
       <c r="D56">
-        <v>0.72934353653198802</v>
+        <v>41.788306458428487</v>
       </c>
       <c r="E56">
-        <f t="shared" si="2"/>
-        <v>0.50553259735944567</v>
+        <v>28.964884234982623</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -9118,17 +9512,16 @@
         <v>11</v>
       </c>
       <c r="B57">
-        <v>0.74490406437344303</v>
+        <v>42.679859030739671</v>
       </c>
       <c r="C57">
-        <v>0.37735710981569698</v>
+        <v>21.620969761694166</v>
       </c>
       <c r="D57">
-        <v>0.81892301523560396</v>
+        <v>46.920832519127721</v>
       </c>
       <c r="E57">
-        <f t="shared" si="2"/>
-        <v>0.64706139647491467</v>
+        <v>37.073887103853856</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -9136,17 +9529,16 @@
         <v>14</v>
       </c>
       <c r="B58">
-        <v>0.80399353499798298</v>
+        <v>46.065436311188066</v>
       </c>
       <c r="C58">
-        <v>0.77505735797830999</v>
+        <v>44.407515492717366</v>
       </c>
       <c r="D58">
-        <v>0.40471685175412803</v>
+        <v>23.188567503333346</v>
       </c>
       <c r="E58">
-        <f t="shared" si="2"/>
-        <v>0.66125591491014035</v>
+        <v>37.88717310241293</v>
       </c>
     </row>
   </sheetData>
@@ -9163,8 +9555,8 @@
   </sheetPr>
   <dimension ref="A1:Y58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView topLeftCell="A55" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12326,10 +12718,1003 @@
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
+  <dimension ref="A1:Q46"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:17">
+      <c r="B1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1" t="s">
+        <v>113</v>
+      </c>
+      <c r="J1" t="s">
+        <v>62</v>
+      </c>
+      <c r="P1">
+        <v>7</v>
+      </c>
+      <c r="Q1">
+        <f>MIN($B$2:$D$46)</f>
+        <v>0.13453294649086753</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2">
+        <v>0.70602565632374648</v>
+      </c>
+      <c r="C2">
+        <v>0.37286313970459789</v>
+      </c>
+      <c r="D2">
+        <v>0.77692475084267687</v>
+      </c>
+      <c r="E2">
+        <v>0.61860451562367369</v>
+      </c>
+      <c r="F2">
+        <f>Q$1 +Q$3 * $M2</f>
+        <v>0.13453294649086753</v>
+      </c>
+      <c r="G2">
+        <f t="array" ref="G2:G10">FREQUENCY(B$2:B$46, $F$2:$F$9)</f>
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <f t="array" ref="H2:H10">FREQUENCY(C$2:C$46, $F$2:$F$9)</f>
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <f t="array" ref="I2:I10">FREQUENCY(D$2:D$46, $F$2:$F$9)</f>
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <f t="array" ref="J2:J10">FREQUENCY(E$2:E$46, $F$2:$F$9)</f>
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <f>MAX($B$2:$D$46)</f>
+        <v>38.709946545061747</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3">
+        <v>0.80724999630765226</v>
+      </c>
+      <c r="C3">
+        <v>1.0341054365134505</v>
+      </c>
+      <c r="D3">
+        <v>0.78883052944532495</v>
+      </c>
+      <c r="E3">
+        <v>0.87672865408880929</v>
+      </c>
+      <c r="F3">
+        <f>Q$1 +Q$3 * $M3</f>
+        <v>5.6453063177152787</v>
+      </c>
+      <c r="G3">
+        <v>37</v>
+      </c>
+      <c r="H3">
+        <v>31</v>
+      </c>
+      <c r="I3">
+        <v>35</v>
+      </c>
+      <c r="J3">
+        <v>34</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <f>(Q2 - Q1) /$P$1</f>
+        <v>5.5107733712244116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4">
+        <v>0.5269495469110983</v>
+      </c>
+      <c r="C4">
+        <v>1.2664799880902653</v>
+      </c>
+      <c r="D4">
+        <v>1.2204449364785015</v>
+      </c>
+      <c r="E4">
+        <v>1.0046248238266215</v>
+      </c>
+      <c r="F4">
+        <f>Q$1 +Q$3 * $M4</f>
+        <v>11.156079688939691</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>7</v>
+      </c>
+      <c r="I4">
+        <v>5</v>
+      </c>
+      <c r="J4">
+        <v>6</v>
+      </c>
+      <c r="M4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5">
+        <v>0.91217940635197847</v>
+      </c>
+      <c r="C5">
+        <v>1.2516911666435977</v>
+      </c>
+      <c r="D5">
+        <v>1.5279714090640786</v>
+      </c>
+      <c r="E5">
+        <v>1.2306139940198848</v>
+      </c>
+      <c r="F5">
+        <f>Q$1 +Q$3 * $M5</f>
+        <v>16.666853060164105</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <v>5</v>
+      </c>
+      <c r="J5">
+        <v>3</v>
+      </c>
+      <c r="M5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6">
+        <v>1.1966620499150127</v>
+      </c>
+      <c r="C6">
+        <v>1.466626932643696</v>
+      </c>
+      <c r="D6">
+        <v>1.4108854452912651</v>
+      </c>
+      <c r="E6">
+        <v>1.3580581426166582</v>
+      </c>
+      <c r="F6">
+        <f>Q$1 +Q$3 * $M6</f>
+        <v>22.177626431388514</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7">
+        <v>1.8801232841853159</v>
+      </c>
+      <c r="C7">
+        <v>0.76988569789867112</v>
+      </c>
+      <c r="D7">
+        <v>1.7155975277253235</v>
+      </c>
+      <c r="E7">
+        <v>1.4552021699364368</v>
+      </c>
+      <c r="F7">
+        <f>Q$1 +Q$3 * $M7</f>
+        <v>27.688399802612924</v>
+      </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8">
+        <v>0.13453294649086753</v>
+      </c>
+      <c r="C8">
+        <v>2.2554282947891311</v>
+      </c>
+      <c r="D8">
+        <v>2.2528861841648062</v>
+      </c>
+      <c r="E8">
+        <v>1.5476158084816014</v>
+      </c>
+      <c r="F8">
+        <f>Q$1 +Q$3 * $M8</f>
+        <v>33.199173173837337</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9">
+        <v>1.9676204430765123</v>
+      </c>
+      <c r="C9">
+        <v>1.8501645086735712</v>
+      </c>
+      <c r="D9">
+        <v>0.95610130930850945</v>
+      </c>
+      <c r="E9">
+        <v>1.5912954203528644</v>
+      </c>
+      <c r="F9">
+        <f>Q$1 +Q$3 * $M9</f>
+        <v>38.709946545061747</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B10">
+        <v>1.2048576169200091</v>
+      </c>
+      <c r="C10">
+        <v>2.2591511628989247</v>
+      </c>
+      <c r="D10">
+        <v>1.9232968038350315</v>
+      </c>
+      <c r="E10">
+        <v>1.7957685278846554</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B11">
+        <v>1.3456371417049053</v>
+      </c>
+      <c r="C11">
+        <v>2.1524825657818494</v>
+      </c>
+      <c r="D11">
+        <v>2.3059724465598461</v>
+      </c>
+      <c r="E11">
+        <v>1.9346973846822002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12">
+        <v>2.4378413387564217</v>
+      </c>
+      <c r="C12">
+        <v>1.4365879195934923</v>
+      </c>
+      <c r="D12">
+        <v>1.976702439323677</v>
+      </c>
+      <c r="E12">
+        <v>1.9503772325578634</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="A13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13">
+        <v>2.6426527641595876</v>
+      </c>
+      <c r="C13">
+        <v>1.7640865636538721</v>
+      </c>
+      <c r="D13">
+        <v>1.9739952057433363</v>
+      </c>
+      <c r="E13">
+        <v>2.1269115111855985</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="A14" t="s">
+        <v>98</v>
+      </c>
+      <c r="B14">
+        <v>0.41640204831153038</v>
+      </c>
+      <c r="C14">
+        <v>2.9848066524769137</v>
+      </c>
+      <c r="D14">
+        <v>3.0135543470864423</v>
+      </c>
+      <c r="E14">
+        <v>2.1382543492916288</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="A15" t="s">
+        <v>99</v>
+      </c>
+      <c r="B15">
+        <v>2.7666577089308122</v>
+      </c>
+      <c r="C15">
+        <v>2.9314641460299167</v>
+      </c>
+      <c r="D15">
+        <v>1.1985030817966866</v>
+      </c>
+      <c r="E15">
+        <v>2.2988749789191387</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="A16" t="s">
+        <v>100</v>
+      </c>
+      <c r="B16">
+        <v>2.6591341045143144</v>
+      </c>
+      <c r="C16">
+        <v>3.01777229937424</v>
+      </c>
+      <c r="D16">
+        <v>1.4903174745230654</v>
+      </c>
+      <c r="E16">
+        <v>2.3890746261372069</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17">
+        <v>1.9376986611277673</v>
+      </c>
+      <c r="C17">
+        <v>3.0369599142134076</v>
+      </c>
+      <c r="D17">
+        <v>2.3388809621008018</v>
+      </c>
+      <c r="E17">
+        <v>2.4378465124806592</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>90</v>
+      </c>
+      <c r="B18">
+        <v>3.146841617248763</v>
+      </c>
+      <c r="C18">
+        <v>2.7588645161454179</v>
+      </c>
+      <c r="D18">
+        <v>1.6055209527080763</v>
+      </c>
+      <c r="E18">
+        <v>2.5037423620340857</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19">
+        <v>2.9755371867890705</v>
+      </c>
+      <c r="C19">
+        <v>3.5761675352014719</v>
+      </c>
+      <c r="D19">
+        <v>2.0824368552822765</v>
+      </c>
+      <c r="E19">
+        <v>2.878047192424273</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20">
+        <v>0.72438646159210052</v>
+      </c>
+      <c r="C20">
+        <v>4.0844776634258588</v>
+      </c>
+      <c r="D20">
+        <v>4.0620983957945</v>
+      </c>
+      <c r="E20">
+        <v>2.9569875069374865</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B21">
+        <v>4.18105867438031</v>
+      </c>
+      <c r="C21">
+        <v>4.2600488389092819</v>
+      </c>
+      <c r="D21">
+        <v>0.86084465324247106</v>
+      </c>
+      <c r="E21">
+        <v>3.1006507221773543</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22">
+        <v>2.8539994420047594</v>
+      </c>
+      <c r="C22">
+        <v>3.9394448770925763</v>
+      </c>
+      <c r="D22">
+        <v>2.7282552167252456</v>
+      </c>
+      <c r="E22">
+        <v>3.1738998452741938</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>106</v>
+      </c>
+      <c r="B23">
+        <v>4.3699660748006703</v>
+      </c>
+      <c r="C23">
+        <v>4.4156067472524372</v>
+      </c>
+      <c r="D23">
+        <v>1.0088541855314075</v>
+      </c>
+      <c r="E23">
+        <v>3.2648090025281715</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>89</v>
+      </c>
+      <c r="B24">
+        <v>4.4825051112784813</v>
+      </c>
+      <c r="C24">
+        <v>4.5432597132918691</v>
+      </c>
+      <c r="D24">
+        <v>0.81188313773143228</v>
+      </c>
+      <c r="E24">
+        <v>3.2792159874339277</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>96</v>
+      </c>
+      <c r="B25">
+        <v>3.1785926467194936</v>
+      </c>
+      <c r="C25">
+        <v>4.1616693423212956</v>
+      </c>
+      <c r="D25">
+        <v>3.0397084373265444</v>
+      </c>
+      <c r="E25">
+        <v>3.4599901421224444</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>95</v>
+      </c>
+      <c r="B26">
+        <v>3.0403925027994489</v>
+      </c>
+      <c r="C26">
+        <v>4.6285341205679034</v>
+      </c>
+      <c r="D26">
+        <v>3.4930124989360958</v>
+      </c>
+      <c r="E26">
+        <v>3.7206463741011491</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>93</v>
+      </c>
+      <c r="B27">
+        <v>3.0777409556647148</v>
+      </c>
+      <c r="C27">
+        <v>4.641696722787656</v>
+      </c>
+      <c r="D27">
+        <v>3.5644395602301757</v>
+      </c>
+      <c r="E27">
+        <v>3.7612924128941816</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>86</v>
+      </c>
+      <c r="B28">
+        <v>5.258644864834821</v>
+      </c>
+      <c r="C28">
+        <v>5.0159599054418438</v>
+      </c>
+      <c r="D28">
+        <v>1.5920356373336471</v>
+      </c>
+      <c r="E28">
+        <v>3.9555468025367708</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>109</v>
+      </c>
+      <c r="B29">
+        <v>2.494495459458606</v>
+      </c>
+      <c r="C29">
+        <v>4.4392556691882525</v>
+      </c>
+      <c r="D29">
+        <v>5.0866586340066533</v>
+      </c>
+      <c r="E29">
+        <v>4.0068032542178376</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>94</v>
+      </c>
+      <c r="B30">
+        <v>2.7379329507323957</v>
+      </c>
+      <c r="C30">
+        <v>4.4442879448123245</v>
+      </c>
+      <c r="D30">
+        <v>5.1215235948183837</v>
+      </c>
+      <c r="E30">
+        <v>4.1012481634543683</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>80</v>
+      </c>
+      <c r="B31">
+        <v>4.2775625817408098</v>
+      </c>
+      <c r="C31">
+        <v>5.5726641092471416</v>
+      </c>
+      <c r="D31">
+        <v>4.4716267787489219</v>
+      </c>
+      <c r="E31">
+        <v>4.7739511565789572</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>92</v>
+      </c>
+      <c r="B32">
+        <v>4.3218773620190305</v>
+      </c>
+      <c r="C32">
+        <v>4.1272120368946883</v>
+      </c>
+      <c r="D32">
+        <v>5.9717810589678137</v>
+      </c>
+      <c r="E32">
+        <v>4.8069568192938439</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33">
+        <v>4.5569999300376303</v>
+      </c>
+      <c r="C33">
+        <v>5.9963208284504264</v>
+      </c>
+      <c r="D33">
+        <v>3.905992925560116</v>
+      </c>
+      <c r="E33">
+        <v>4.8197712280160578</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>91</v>
+      </c>
+      <c r="B34">
+        <v>3.6905673508188968</v>
+      </c>
+      <c r="C34">
+        <v>6.1191179560720492</v>
+      </c>
+      <c r="D34">
+        <v>5.3696750583625406</v>
+      </c>
+      <c r="E34">
+        <v>5.0597867884178287</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>107</v>
+      </c>
+      <c r="B35">
+        <v>2.5694803198973601</v>
+      </c>
+      <c r="C35">
+        <v>6.3648372913965758</v>
+      </c>
+      <c r="D35">
+        <v>6.7883603474772292</v>
+      </c>
+      <c r="E35">
+        <v>5.2408926529237219</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
+        <v>104</v>
+      </c>
+      <c r="B36">
+        <v>3.0792105331427635</v>
+      </c>
+      <c r="C36">
+        <v>8.6144519022034647</v>
+      </c>
+      <c r="D36">
+        <v>8.3143710814693002</v>
+      </c>
+      <c r="E36">
+        <v>6.6693445056051761</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>105</v>
+      </c>
+      <c r="B37">
+        <v>4.8003390563447974</v>
+      </c>
+      <c r="C37">
+        <v>9.1966592469145461</v>
+      </c>
+      <c r="D37">
+        <v>8.0057961740350727</v>
+      </c>
+      <c r="E37">
+        <v>7.334264825764806</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" t="s">
+        <v>103</v>
+      </c>
+      <c r="B38">
+        <v>9.2789793281278925</v>
+      </c>
+      <c r="C38">
+        <v>10.120423028756917</v>
+      </c>
+      <c r="D38">
+        <v>4.0395278253801798</v>
+      </c>
+      <c r="E38">
+        <v>7.8129767274216633</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
+        <v>87</v>
+      </c>
+      <c r="B39">
+        <v>1.4862989020556667</v>
+      </c>
+      <c r="C39">
+        <v>12.198838080225892</v>
+      </c>
+      <c r="D39">
+        <v>12.107945310336067</v>
+      </c>
+      <c r="E39">
+        <v>8.5976940975392093</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
+        <v>84</v>
+      </c>
+      <c r="B40">
+        <v>1.7662181879611247</v>
+      </c>
+      <c r="C40">
+        <v>12.871656898686179</v>
+      </c>
+      <c r="D40">
+        <v>12.749275877138965</v>
+      </c>
+      <c r="E40">
+        <v>9.1290503212620902</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" t="s">
+        <v>78</v>
+      </c>
+      <c r="B41">
+        <v>10.455750202551174</v>
+      </c>
+      <c r="C41">
+        <v>11.696573664580123</v>
+      </c>
+      <c r="D41">
+        <v>5.2352002036560981</v>
+      </c>
+      <c r="E41">
+        <v>9.1291746902624666</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" t="s">
+        <v>85</v>
+      </c>
+      <c r="B42">
+        <v>15.747907546302615</v>
+      </c>
+      <c r="C42">
+        <v>7.190427391949008</v>
+      </c>
+      <c r="D42">
+        <v>14.897999091595688</v>
+      </c>
+      <c r="E42">
+        <v>12.612111343282438</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" t="s">
+        <v>76</v>
+      </c>
+      <c r="B43">
+        <v>14.2773748909527</v>
+      </c>
+      <c r="C43">
+        <v>16.737116685115989</v>
+      </c>
+      <c r="D43">
+        <v>8.7555710867971808</v>
+      </c>
+      <c r="E43">
+        <v>13.256687554288623</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" t="s">
+        <v>82</v>
+      </c>
+      <c r="B44">
+        <v>22.951983235726946</v>
+      </c>
+      <c r="C44">
+        <v>22.971598277384146</v>
+      </c>
+      <c r="D44">
+        <v>1.1380360427223408</v>
+      </c>
+      <c r="E44">
+        <v>15.687205851944478</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" t="s">
+        <v>83</v>
+      </c>
+      <c r="B45">
+        <v>24.204192794938873</v>
+      </c>
+      <c r="C45">
+        <v>28.060726506120588</v>
+      </c>
+      <c r="D45">
+        <v>14.097535404336213</v>
+      </c>
+      <c r="E45">
+        <v>22.120818235131892</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" t="s">
+        <v>81</v>
+      </c>
+      <c r="B46">
+        <v>38.453997236120614</v>
+      </c>
+      <c r="C46">
+        <v>38.709946545061747</v>
+      </c>
+      <c r="D46">
+        <v>16.069017931893129</v>
+      </c>
+      <c r="E46">
+        <v>31.077653904358499</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <tabColor theme="7" tint="-0.249977111117893"/>
+  </sheetPr>
   <dimension ref="A1:Y46"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E46"/>
+      <selection sqref="A1:E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>